<commit_message>
Updated to larger Llama model
</commit_message>
<xml_diff>
--- a/Results from Eval.xlsx
+++ b/Results from Eval.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\MEng Project\MEng_Project_RAG_for_Defence\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C77DBF8A-382E-4C08-8B67-4D7238EA9512}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1F07F48-51E7-4B1B-91C4-B75E761C9745}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" xr2:uid="{34AF9B4A-10A5-43EE-9A56-6B315E5937F1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Model Change</t>
   </si>
@@ -54,6 +54,15 @@
   </si>
   <si>
     <t>Semantic Chunker</t>
+  </si>
+  <si>
+    <t>BM25 Retriever + Semantic chunking</t>
+  </si>
+  <si>
+    <t>BM25 Retriever + Semantic chunking + Llama 3.2:3B</t>
+  </si>
+  <si>
+    <t>BM25 Retriever + Semantic chunking + Llama 3.2:3B + Prompt Templates</t>
   </si>
 </sst>
 </file>
@@ -425,15 +434,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6ECF7A9-1D4E-4ED4-A50A-87A0E31FAC3A}">
-  <dimension ref="A2:D4"/>
+  <dimension ref="A2:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="65" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
@@ -481,6 +490,39 @@
         <v>0.1772</v>
       </c>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>0.73380000000000001</v>
+      </c>
+      <c r="C5">
+        <v>0.53300000000000003</v>
+      </c>
+      <c r="D5">
+        <v>0.18210000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>0.76749999999999996</v>
+      </c>
+      <c r="C6">
+        <v>0.57220000000000004</v>
+      </c>
+      <c r="D6">
+        <v>0.24779999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>